<commit_message>
File Upload fixed and ES6 support included
</commit_message>
<xml_diff>
--- a/webapp/src/PartnerTemplate.xlsx
+++ b/webapp/src/PartnerTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalibor.riger\Downloads\eclipse\serverworkspace\dr\driger\OrionContent\ZAKV_CDV\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalibor.riger\Downloads\eclipse\serverworkspace\dr\driger\OrionContent\bp\webapp\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24694" windowHeight="9634"/>
   </bookViews>
   <sheets>
     <sheet name="Partner" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>Email</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Titula</t>
   </si>
   <si>
-    <t>Naziv</t>
-  </si>
-  <si>
-    <t>Naziv 2</t>
-  </si>
-  <si>
     <t>Naziv 3</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t>Grad</t>
   </si>
   <si>
-    <t>Zemlja</t>
-  </si>
-  <si>
     <t>Mobitel</t>
   </si>
   <si>
@@ -220,6 +211,30 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>Ime</t>
+  </si>
+  <si>
+    <t>Prezim</t>
+  </si>
+  <si>
+    <t>Firma</t>
+  </si>
+  <si>
+    <t>Ostatak</t>
+  </si>
+  <si>
+    <t>Prezime</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Zaglavlje</t>
+  </si>
+  <si>
+    <t>Header_Agent</t>
   </si>
 </sst>
 </file>
@@ -236,7 +251,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +270,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -268,11 +289,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,147 +585,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AK4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" outlineLevelCol="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="15" width="9.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="13.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="14.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="16.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="16.85546875" customWidth="1"/>
-    <col min="21" max="21" width="13.28515625" customWidth="1"/>
-    <col min="38" max="38" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.23046875" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="15" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="23.53515625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="7" width="13.3828125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="9.4609375" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="10" width="13.23046875" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="12.3046875" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="12.15234375" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="18.3046875" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="16" width="9.3046875" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="13.3046875" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="10.84375" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="14.3828125" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="16.84375" customWidth="1"/>
+    <col min="21" max="21" width="13.3046875" customWidth="1"/>
+    <col min="22" max="23" width="13.3828125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" hidden="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
+        <v>60</v>
+      </c>
+      <c r="U1" t="s">
         <v>40</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
         <v>41</v>
       </c>
-      <c r="S1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>43</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>44</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>45</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>52</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>53</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>54</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>55</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -722,7 +756,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
@@ -741,137 +775,133 @@
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
       <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" t="s">
+      <c r="R3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" t="s">
         <v>12</v>
       </c>
-      <c r="N3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" t="s">
-        <v>16</v>
-      </c>
       <c r="T3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="U3" t="s">
         <v>1</v>
       </c>
       <c r="V3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" t="s">
+        <v>66</v>
+      </c>
+      <c r="X3" t="s">
         <v>2</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>3</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>4</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB3" t="s">
         <v>5</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AC3" t="s">
         <v>6</v>
       </c>
-      <c r="AA3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB3" t="s">
+      <c r="AD3" t="s">
         <v>7</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG3" t="s">
         <v>8</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>11</v>
       </c>
       <c r="AH3" t="s">
         <v>0</v>
       </c>
       <c r="AI3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AJ3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AK3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
       <c r="U4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="2">
-    <mergeCell ref="A2:S2"/>
-    <mergeCell ref="T2:AL2"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="T2:AK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -882,7 +912,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>U4:U38 B4:B50</xm:sqref>
+          <xm:sqref>U4:U38 C4:C50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -898,208 +928,208 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="E16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" t="s">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" t="s">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.4">
+      <c r="E36" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>